<commit_message>
Integrate Whole Foods order data with complete store and item mapping
Implements the Whole Foods parser with store/item mapping XLSX files and adds a store list as attached_assets/Pasted-StoreNo-CustomerId-AccountNumber-CompanyName-ShipToCompanyName-10005-4374-1508-WHOLE-FOODS-10005-P-1753745293745_1753745293747.txt.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a4c793ea-64cf-4601-8936-3568869ffe5a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/c5fd0f16-2d84-4af3-99b4-3191adee6a6a/a4c793ea-64cf-4601-8936-3568869ffe5a/P4K1CYm
</commit_message>
<xml_diff>
--- a/mappings/wholefoods/store_mapping.xlsx
+++ b/mappings/wholefoods/store_mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,72 +448,612 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Whole Foods Market - Downtown</t>
+          <t>WHOLE FOODS #10005 PALO ALTO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Whole Foods Downtown</t>
+          <t>WHOLE FOODS #10005 PALO ALTO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Whole Foods Market - Uptown</t>
+          <t>WHOLE FOODS #10006 TELEGRAPH</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Whole Foods Uptown</t>
+          <t>WHOLE FOODS #10006 TELEGRAPH</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Whole Foods Market - West Side</t>
+          <t>WHOLE FOODS #10009 MILLER</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Whole Foods West Side</t>
+          <t>WHOLE FOODS #10009 MILLER</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>WFM Central</t>
+          <t>WHOLE FOODS #10027 LOS GATOS</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Whole Foods Central</t>
+          <t>WHOLE FOODS #10027 LOS GATOS</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Whole Foods - Main Street</t>
+          <t>WHOLE FOODS #10033 CAMPBELL</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Whole Foods Main Street</t>
+          <t>WHOLE FOODS #10033 CAMPBELL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sample Store Name</t>
+          <t>WHOLE FOODS #10044 SF CALI ST</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mapped Store Name</t>
+          <t>WHOLE FOODS #10044 SF CALI ST</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10071 SAN RAFAEL</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10071 SAN RAFAEL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10087 MONTEREY</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10087 MONTEREY</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10101 WALNUT CREEK</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10101 WALNUT CREEK</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10122 FRESNO</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10122 FRESNO</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10126 SAN RAMON</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10126 SAN RAMON</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10137 SEBASTOPOL</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10137 SEBASTOPOL</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10138 PETALUMA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10138 PETALUMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10139 YULUPA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10139 YULUPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10150 SAN MATEO</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10150 SAN MATEO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10151 SF 4TH ST</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10151 SF 4TH ST</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10152 SACRAMENTO</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10152 SACRAMENTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10154 REDWOOD CITY</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10154 REDWOOD CITY</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10155 LOS ALTOS</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10155 LOS ALTOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10221 HARRISON</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10221 HARRISON</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10230 ROSEVILLE</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10230 ROSEVILLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10234 NOVATO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10234 NOVATO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10238 SF RHODE</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10238 SF RHODE</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10259 SAN JOSE</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10259 SAN JOSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10267 CUPERTINO</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10267 CUPERTINO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10281 SONOMA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10281 SONOMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10284 BOISE</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10284 BOISE</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10288 NAPA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10288 NAPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10293 RENO</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10293 RENO</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10320 SAN JOSE</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10320 SAN JOSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10329 SANTA CRUZ</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10329 SANTA CRUZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10337 BLITHEDALE</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10337 BLITHEDALE</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10349 LAFAYETTE</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10349 LAFAYETTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10362 SF STANYON</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10362 SF STANYON</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10365 CAPITOLA</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10365 CAPITOLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10370 CODDINGTOWN</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10370 CODDINGTOWN</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10379 SF 24TH ST</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10379 SF 24TH ST</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10396 CASTRO</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10396 CASTRO</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10432 SF OCEAN</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10432 SF OCEAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10447 FOLSOM</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10447 FOLSOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10467 FREMONT</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10467 FREMONT</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10530 GILMAN ST</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10530 GILMAN ST</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10547 DUBLIN</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10547 DUBLIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10548 YVR</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10548 YVR</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10633 SANTA CLARA</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10633 SANTA CLARA</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10677 CONCORD</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10677 CONCORD</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10703 TAHOE</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10703 TAHOE</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10707 SUNNYVALE</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10707 SUNNYVALE</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10708 TEMESCAL</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10708 TEMESCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10717 STONESTOWN</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10717 STONESTOWN</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10718 TRINITY</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>WHOLE FOODS #10718 TRINITY</t>
         </is>
       </c>
     </row>

</xml_diff>